<commit_message>
modified readme.md file and made a few changes
</commit_message>
<xml_diff>
--- a/src/test/resources/WebFormTestCase.xlsx
+++ b/src/test/resources/WebFormTestCase.xlsx
@@ -1,19 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9A7145FC-8382-477A-881C-34107A75FE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="19665" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="19665" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -318,18 +316,6 @@
     <t>qwerty</t>
   </si>
   <si>
-    <t>rohit93m@gmail.com</t>
-  </si>
-  <si>
-    <t>rohit93m@yahoo.com</t>
-  </si>
-  <si>
-    <t>rohit93m@rediff.com</t>
-  </si>
-  <si>
-    <t>rohit@gmail.com</t>
-  </si>
-  <si>
     <t>qwer1</t>
   </si>
   <si>
@@ -345,12 +331,6 @@
     <t>qwer@1234</t>
   </si>
   <si>
-    <t>rohit93m@@gmail.com</t>
-  </si>
-  <si>
-    <t>rohit93m@gmail</t>
-  </si>
-  <si>
     <t>qwert1</t>
   </si>
   <si>
@@ -358,13 +338,31 @@
   </si>
   <si>
     <t>email id</t>
+  </si>
+  <si>
+    <t>abc123@gmail.com</t>
+  </si>
+  <si>
+    <t>abc123@yahoo.com</t>
+  </si>
+  <si>
+    <t>abc123@rediff.com</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>abc123@@gmail.com</t>
+  </si>
+  <si>
+    <t>abc123@gmail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,21 +719,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
@@ -746,7 +744,7 @@
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="8" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -769,7 +767,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -786,7 +784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="C3" s="4" t="s">
         <v>70</v>
       </c>
@@ -797,7 +795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="C4" s="4" t="s">
         <v>71</v>
       </c>
@@ -808,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="C5" s="4" t="s">
         <v>72</v>
       </c>
@@ -819,7 +817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="C6" s="4" t="s">
         <v>73</v>
       </c>
@@ -830,7 +828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="C7" s="4" t="s">
         <v>80</v>
       </c>
@@ -841,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="C8" s="4" t="s">
         <v>74</v>
       </c>
@@ -852,7 +850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="C9" s="4" t="s">
         <v>75</v>
       </c>
@@ -860,7 +858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -877,7 +875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
@@ -888,7 +886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
@@ -899,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="C14" s="4" t="s">
         <v>79</v>
       </c>
@@ -910,7 +908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
@@ -921,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
@@ -932,7 +930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
@@ -943,7 +941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
@@ -951,7 +949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -968,7 +966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="C21" s="4" t="s">
         <v>18</v>
       </c>
@@ -979,29 +977,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="C23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16.5">
       <c r="C24" s="4" t="s">
         <v>21</v>
       </c>
@@ -1012,7 +1010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="C25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1020,7 +1018,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>4</v>
       </c>
@@ -1031,24 +1029,24 @@
         <v>24</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="C28" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="C29" s="4" t="s">
         <v>26</v>
       </c>
@@ -1059,18 +1057,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="16.5">
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
@@ -1081,7 +1079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="C32" s="4" t="s">
         <v>29</v>
       </c>
@@ -1089,7 +1087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>5</v>
       </c>
@@ -1106,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="C35" s="4" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>6</v>
       </c>
@@ -1125,13 +1123,13 @@
         <v>36</v>
       </c>
       <c r="D37" s="3">
-        <v>560071</v>
+        <v>110010</v>
       </c>
       <c r="E37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="C38" s="4" t="s">
         <v>37</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="C39" s="4" t="s">
         <v>38</v>
       </c>
@@ -1153,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="16.5">
       <c r="C40" s="4" t="s">
         <v>39</v>
       </c>
@@ -1164,7 +1162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="C41" s="4" t="s">
         <v>40</v>
       </c>
@@ -1172,29 +1170,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="C42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="C43" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="C44" s="4" t="s">
         <v>43</v>
       </c>
@@ -1205,46 +1203,46 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>7</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="C47" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="C48" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E48" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="C49" s="4" t="s">
         <v>48</v>
       </c>
@@ -1255,18 +1253,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="C50" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="C51" s="4" t="s">
         <v>51</v>
       </c>
@@ -1274,7 +1272,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="16.5">
       <c r="C52" s="4" t="s">
         <v>52</v>
       </c>
@@ -1285,29 +1283,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="C53" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E53" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="C54" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="2">
         <v>8</v>
       </c>
@@ -1324,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="C57" s="4" t="s">
         <v>58</v>
       </c>
@@ -1335,7 +1333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="C58" s="4" t="s">
         <v>59</v>
       </c>
@@ -1343,7 +1341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" s="2">
         <v>9</v>
       </c>
@@ -1360,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="C61" s="4" t="s">
         <v>64</v>
       </c>
@@ -1371,7 +1369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="C62" s="4" t="s">
         <v>59</v>
       </c>
@@ -1381,18 +1379,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" display="adf@4" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D23" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D44" r:id="rId4" display="asdf@4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D43" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D46" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D47" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D48" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D49" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D54" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D50" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D30" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D8" r:id="rId1" display="adf@4"/>
+    <hyperlink ref="D15" r:id="rId2"/>
+    <hyperlink ref="D23" r:id="rId3"/>
+    <hyperlink ref="D44" r:id="rId4" display="asdf@4"/>
+    <hyperlink ref="D43" r:id="rId5"/>
+    <hyperlink ref="D46" r:id="rId6"/>
+    <hyperlink ref="D47" r:id="rId7"/>
+    <hyperlink ref="D48" r:id="rId8"/>
+    <hyperlink ref="D49" r:id="rId9"/>
+    <hyperlink ref="D54" r:id="rId10"/>
+    <hyperlink ref="D50" r:id="rId11"/>
+    <hyperlink ref="D30" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>